<commit_message>
Irfan - Submitting some previous results
</commit_message>
<xml_diff>
--- a/goldendata/Assignment2Part1Comparison/Assignment2Part1Comparison.xlsx
+++ b/goldendata/Assignment2Part1Comparison/Assignment2Part1Comparison.xlsx
@@ -3018,7 +3018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
@@ -3967,6 +3967,7 @@
     <mergeCell ref="N11:O11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>